<commit_message>
updated AO data (10.19.2015) and recalcuated and reported
</commit_message>
<xml_diff>
--- a/province2015/pre-proc/2_AO/6B_ao_afc.xlsx
+++ b/province2015/pre-proc/2_AO/6B_ao_afc.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="200" windowWidth="14800" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -58,7 +63,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>individual</t>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -66,13 +71,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="164" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -84,14 +89,14 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -123,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,15 +136,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -441,17 +443,17 @@
   <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="9" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="15.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -462,1340 +464,1345 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>2003</v>
       </c>
-      <c r="C2" s="4">
-        <v>182376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C2" s="3">
+        <v>86.680608365019012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2004</v>
       </c>
-      <c r="C3" s="4">
-        <v>178996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C3" s="3">
+        <v>85.07414448669202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>2005</v>
       </c>
-      <c r="C4" s="4">
-        <v>202298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C4" s="3">
+        <v>96.149239543726239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>2006</v>
       </c>
-      <c r="C5" s="4">
-        <v>185541</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C5" s="3">
+        <v>88.184885931558938</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>2007</v>
       </c>
-      <c r="C6" s="4">
-        <v>179061</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C6" s="3">
+        <v>85.105038022813687</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>2008</v>
       </c>
-      <c r="C7" s="4">
-        <v>304610</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" s="3">
+        <v>144.77661596958174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>2009</v>
       </c>
-      <c r="C8" s="4">
-        <v>312272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C8" s="3">
+        <v>148.41825095057035</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>2010</v>
       </c>
-      <c r="C9" s="4">
-        <v>286158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C9" s="3">
+        <v>136.00665399239543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>2011</v>
       </c>
-      <c r="C10" s="4">
-        <v>320704</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C10" s="3">
+        <v>152.42585551330799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>2012</v>
       </c>
-      <c r="C11" s="4">
-        <v>317448</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C11" s="3">
+        <v>150.87832699619773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>2013</v>
       </c>
-      <c r="C12" s="4">
-        <v>313506</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C12" s="3">
+        <v>149.00475285171103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>2003</v>
       </c>
-      <c r="C13" s="4">
-        <v>102198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C13" s="3">
+        <v>210.78271630401153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1">
         <v>2004</v>
       </c>
-      <c r="C14" s="4">
-        <v>102827</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C14" s="3">
+        <v>212.08002474992264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>2005</v>
       </c>
-      <c r="C15" s="4">
-        <v>112740</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C15" s="3">
+        <v>232.5255233577395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1">
         <v>2006</v>
       </c>
-      <c r="C16" s="4">
-        <v>112727</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C16" s="3">
+        <v>232.49871094152829</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1">
         <v>2007</v>
       </c>
-      <c r="C17" s="4">
-        <v>85539</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C17" s="3">
+        <v>176.42363617613694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="1">
         <v>2008</v>
       </c>
-      <c r="C18" s="4">
-        <v>114156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C18" s="3">
+        <v>235.44601423120551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>2009</v>
       </c>
-      <c r="C19" s="4">
-        <v>113071</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C19" s="3">
+        <v>233.20820872434771</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>2010</v>
       </c>
-      <c r="C20" s="4">
-        <v>110178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C20" s="3">
+        <v>227.24141487057852</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1">
         <v>2011</v>
       </c>
-      <c r="C21" s="4">
-        <v>113485</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C21" s="3">
+        <v>234.06208105599669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="1">
         <v>2012</v>
       </c>
-      <c r="C22" s="4">
-        <v>116612</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C22" s="3">
+        <v>240.51149840156748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1">
         <v>2013</v>
       </c>
-      <c r="C23" s="4">
-        <v>117403</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C23" s="3">
+        <v>242.14293080334122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="1">
         <v>2003</v>
       </c>
-      <c r="C24" s="4">
-        <v>7149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C24" s="3">
+        <v>46.52176742370014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="1">
         <v>2004</v>
       </c>
-      <c r="C25" s="4">
-        <v>7399</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C25" s="3">
+        <v>48.148630181557891</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="1">
         <v>2005</v>
       </c>
-      <c r="C26" s="4">
-        <v>11601</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C26" s="3">
+        <v>75.4929394156309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="1">
         <v>2006</v>
       </c>
-      <c r="C27" s="4">
-        <v>11359</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C27" s="3">
+        <v>73.918136266024604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="1">
         <v>2007</v>
       </c>
-      <c r="C28" s="4">
-        <v>11280</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C28" s="3">
+        <v>73.404047634541556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="1">
         <v>2008</v>
       </c>
-      <c r="C29" s="4">
-        <v>16954</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C29" s="3">
+        <v>110.32732478688099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="1">
         <v>2009</v>
       </c>
-      <c r="C30" s="4">
-        <v>8191</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C30" s="3">
+        <v>53.302531398451229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1">
         <v>2010</v>
       </c>
-      <c r="C31" s="4">
-        <v>9033</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C31" s="3">
+        <v>58.781805166916122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1">
         <v>2011</v>
       </c>
-      <c r="C32" s="4">
-        <v>8713</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C32" s="3">
+        <v>56.699420836858209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1">
         <v>2012</v>
       </c>
-      <c r="C33" s="4">
-        <v>7264</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C33" s="3">
+        <v>47.270124292314705</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1">
         <v>2013</v>
       </c>
-      <c r="C34" s="4">
-        <v>7264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C34" s="3">
+        <v>47.270124292314705</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="1">
         <v>2003</v>
       </c>
-      <c r="C35" s="4">
-        <v>622899</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C35" s="3">
+        <v>186.19511509799995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1">
         <v>2004</v>
       </c>
-      <c r="C36" s="4">
-        <v>577767</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C36" s="3">
+        <v>172.7043919878281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="1">
         <v>2005</v>
       </c>
-      <c r="C37" s="4">
-        <v>550788</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C37" s="3">
+        <v>164.63990960749206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1">
         <v>2006</v>
       </c>
-      <c r="C38" s="4">
-        <v>446725</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C38" s="3">
+        <v>133.53370737816891</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B39" s="1">
         <v>2007</v>
       </c>
-      <c r="C39" s="4">
-        <v>413203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C39" s="3">
+        <v>123.51341091226487</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1">
         <v>2008</v>
       </c>
-      <c r="C40" s="4">
-        <v>444418</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C40" s="3">
+        <v>132.84410580466968</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1">
         <v>2009</v>
       </c>
-      <c r="C41" s="4">
-        <v>438524</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C41" s="3">
+        <v>131.08228886743331</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="1">
         <v>2010</v>
       </c>
-      <c r="C42" s="4">
-        <v>470307</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C42" s="3">
+        <v>140.58276862925621</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1">
         <v>2011</v>
       </c>
-      <c r="C43" s="4">
-        <v>448007</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C43" s="3">
+        <v>133.91691900245411</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="1">
         <v>2012</v>
       </c>
-      <c r="C44" s="4">
-        <v>402658</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C44" s="3">
+        <v>120.36133089815598</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="1">
         <v>2013</v>
       </c>
-      <c r="C45" s="4">
-        <v>394337</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C45" s="3">
+        <v>117.87404234458558</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="1">
         <v>2003</v>
       </c>
-      <c r="C46" s="4">
-        <v>128682</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C46" s="3">
+        <v>144.75811214417089</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="1">
         <v>2004</v>
       </c>
-      <c r="C47" s="4">
-        <v>127919</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C47" s="3">
+        <v>143.89979132567257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="1">
         <v>2005</v>
       </c>
-      <c r="C48" s="4">
-        <v>119029</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C48" s="3">
+        <v>133.89917261472868</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="1">
         <v>2006</v>
       </c>
-      <c r="C49" s="4">
-        <v>118015</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C49" s="3">
+        <v>132.75849462002711</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="1">
         <v>2007</v>
       </c>
-      <c r="C50" s="4">
-        <v>123830</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C50" s="3">
+        <v>139.29995669023393</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="1">
         <v>2008</v>
       </c>
-      <c r="C51" s="4">
-        <v>137772</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C51" s="3">
+        <v>154.98371665288627</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="1">
         <v>2009</v>
       </c>
-      <c r="C52" s="4">
-        <v>122820</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C52" s="3">
+        <v>138.16377841148775</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="1">
         <v>2010</v>
       </c>
-      <c r="C53" s="4">
-        <v>125386</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C53" s="3">
+        <v>141.0503461968963</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="1">
         <v>2011</v>
       </c>
-      <c r="C54" s="4">
-        <v>110802</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C54" s="3">
+        <v>124.6443818233974</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="1">
         <v>2012</v>
       </c>
-      <c r="C55" s="4">
-        <v>98063</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C55" s="3">
+        <v>110.3139114343407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="1">
         <v>2013</v>
       </c>
-      <c r="C56" s="4">
-        <v>95236</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C56" s="3">
+        <v>107.13373718284032</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="1">
         <v>2003</v>
       </c>
-      <c r="C57" s="4">
-        <v>3339</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C57" s="3">
+        <v>15.824644549763033</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="1">
         <v>2004</v>
       </c>
-      <c r="C58" s="4">
-        <v>3312</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C58" s="3">
+        <v>15.696682464454977</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1">
         <v>2005</v>
       </c>
-      <c r="C59" s="4">
-        <v>4855</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C59" s="3">
+        <v>23.009478672985782</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B60" s="1">
         <v>2006</v>
       </c>
-      <c r="C60" s="4">
-        <v>6650</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C60" s="3">
+        <v>31.51658767772512</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B61" s="1">
         <v>2007</v>
       </c>
-      <c r="C61" s="4">
-        <v>4947</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C61" s="3">
+        <v>23.445497630331754</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B62" s="1">
         <v>2008</v>
       </c>
-      <c r="C62" s="4">
-        <v>5053</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C62" s="3">
+        <v>23.947867298578199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B63" s="1">
         <v>2009</v>
       </c>
-      <c r="C63" s="4">
-        <v>4929</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C63" s="3">
+        <v>23.360189573459717</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B64" s="1">
         <v>2010</v>
       </c>
-      <c r="C64" s="4">
-        <v>4980</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C64" s="3">
+        <v>23.601895734597157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B65" s="1">
         <v>2011</v>
       </c>
-      <c r="C65" s="4">
-        <v>4771</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C65" s="3">
+        <v>22.611374407582939</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B66" s="1">
         <v>2012</v>
       </c>
-      <c r="C66" s="4">
-        <v>4909</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C66" s="3">
+        <v>23.265402843601894</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B67" s="1">
         <v>2013</v>
       </c>
-      <c r="C67" s="4">
-        <v>4027</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C67" s="3">
+        <v>19.085308056872037</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="1">
         <v>2003</v>
       </c>
-      <c r="C68" s="4">
-        <v>452461</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C68" s="3">
+        <v>203.99899547195912</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="1">
         <v>2004</v>
       </c>
-      <c r="C69" s="4">
-        <v>383297</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C69" s="3">
+        <v>172.81534312883434</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="1">
         <v>2005</v>
       </c>
-      <c r="C70" s="4">
-        <v>324398</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C70" s="3">
+        <v>146.25982379279671</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="1">
         <v>2006</v>
       </c>
-      <c r="C71" s="4">
-        <v>325750</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C71" s="3">
+        <v>146.86939377093424</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B72" s="1">
         <v>2007</v>
       </c>
-      <c r="C72" s="4">
-        <v>334746</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C72" s="3">
+        <v>150.92537862546479</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="1">
         <v>2008</v>
       </c>
-      <c r="C73" s="4">
-        <v>317109</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C73" s="3">
+        <v>142.97346612220164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="1">
         <v>2009</v>
       </c>
-      <c r="C74" s="4">
-        <v>309267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C74" s="3">
+        <v>139.43777990285656</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B75" s="1">
         <v>2010</v>
       </c>
-      <c r="C75" s="4">
-        <v>337878</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C75" s="3">
+        <v>152.3374889594343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="1">
         <v>2011</v>
       </c>
-      <c r="C76" s="4">
-        <v>326781</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C76" s="3">
+        <v>147.33423596580096</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="1">
         <v>2012</v>
       </c>
-      <c r="C77" s="4">
-        <v>324034</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C77" s="3">
+        <v>146.09570879868275</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="1">
         <v>2013</v>
       </c>
-      <c r="C78" s="4">
-        <v>319559</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C78" s="3">
+        <v>144.07808627489172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="1">
         <v>2003</v>
       </c>
-      <c r="C79" s="4">
-        <v>870018</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C79" s="3">
+        <v>249.57487091222032</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="1">
         <v>2004</v>
       </c>
-      <c r="C80" s="4">
-        <v>902792</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C80" s="3">
+        <v>258.97647733792314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="1">
         <v>2005</v>
       </c>
-      <c r="C81" s="4">
-        <v>877543</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C81" s="3">
+        <v>251.73350545037292</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="1">
         <v>2006</v>
       </c>
-      <c r="C82" s="4">
-        <v>837435</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C82" s="3">
+        <v>240.22805507745267</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="1">
         <v>2007</v>
       </c>
-      <c r="C83" s="4">
-        <v>853808</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C83" s="3">
+        <v>244.92484222604705</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="1">
         <v>2008</v>
       </c>
-      <c r="C84" s="4">
-        <v>901395</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C84" s="3">
+        <v>258.57573149741825</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="1">
         <v>2009</v>
       </c>
-      <c r="C85" s="4">
-        <v>892096</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C85" s="3">
+        <v>255.90820424555363</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="1">
         <v>2010</v>
       </c>
-      <c r="C86" s="4">
-        <v>834869</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C86" s="3">
+        <v>239.49196787148594</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="1">
         <v>2011</v>
       </c>
-      <c r="C87" s="4">
-        <v>827615</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C87" s="3">
+        <v>237.4110728628801</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="1">
         <v>2012</v>
       </c>
-      <c r="C88" s="4">
-        <v>818372</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C88" s="3">
+        <v>234.75960986804361</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="1">
         <v>2013</v>
       </c>
-      <c r="C89" s="4">
-        <v>818839</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C89" s="3">
+        <v>234.89357429718876</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B90" s="1">
         <v>2003</v>
       </c>
-      <c r="C90" s="4">
-        <v>671426</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C90" s="3">
+        <v>167.21522959450508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B91" s="1">
         <v>2004</v>
       </c>
-      <c r="C91" s="4">
-        <v>660120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C91" s="3">
+        <v>164.3995278108454</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B92" s="1">
         <v>2005</v>
       </c>
-      <c r="C92" s="4">
-        <v>652658</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C92" s="3">
+        <v>162.54115467183351</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B93" s="1">
         <v>2006</v>
       </c>
-      <c r="C93" s="4">
-        <v>664033</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C93" s="3">
+        <v>165.37404055447359</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B94" s="1">
         <v>2007</v>
       </c>
-      <c r="C94" s="4">
-        <v>650178</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C94" s="3">
+        <v>161.92352328818978</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B95" s="1">
         <v>2008</v>
       </c>
-      <c r="C95" s="4">
-        <v>707087</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C95" s="3">
+        <v>176.09642022842399</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B96" s="1">
         <v>2009</v>
       </c>
-      <c r="C96" s="4">
-        <v>707445</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C96" s="3">
+        <v>176.18557830719192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B97" s="1">
         <v>2010</v>
       </c>
-      <c r="C97" s="4">
-        <v>720967</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C97" s="3">
+        <v>179.55316361752679</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B98" s="1">
         <v>2011</v>
       </c>
-      <c r="C98" s="4">
-        <v>718351</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C98" s="3">
+        <v>178.90166212574775</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B99" s="1">
         <v>2012</v>
       </c>
-      <c r="C99" s="4">
-        <v>719572</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C99" s="3">
+        <v>179.20574596422719</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B100" s="1">
         <v>2013</v>
       </c>
-      <c r="C100" s="4">
-        <v>710003</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C100" s="3">
+        <v>176.82263519403088</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B101" s="1">
         <v>2003</v>
       </c>
-      <c r="C101" s="4">
-        <v>119777</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C101" s="3">
+        <v>73.546442014257735</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B102" s="1">
         <v>2004</v>
       </c>
-      <c r="C102" s="4">
-        <v>105018</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C102" s="3">
+        <v>64.484001498228537</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B103" s="1">
         <v>2005</v>
       </c>
-      <c r="C103" s="4">
-        <v>105397</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C103" s="3">
+        <v>64.716718142687853</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B104" s="1">
         <v>2006</v>
       </c>
-      <c r="C104" s="4">
-        <v>114224</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C104" s="3">
+        <v>70.136744054673059</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B105" s="1">
         <v>2007</v>
       </c>
-      <c r="C105" s="4">
-        <v>114405</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C105" s="3">
+        <v>70.247883138174743</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B106" s="1">
         <v>2008</v>
       </c>
-      <c r="C106" s="4">
-        <v>113200</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C106" s="3">
+        <v>69.507979294972955</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B107" s="1">
         <v>2009</v>
       </c>
-      <c r="C107" s="4">
-        <v>112000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C107" s="3">
+        <v>68.771145592199389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B108" s="1">
         <v>2010</v>
       </c>
-      <c r="C108" s="4">
-        <v>112061</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C108" s="3">
+        <v>68.808601305423707</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B109" s="1">
         <v>2011</v>
       </c>
-      <c r="C109" s="4">
-        <v>87485</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C109" s="3">
+        <v>53.718247072621104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B110" s="1">
         <v>2012</v>
       </c>
-      <c r="C110" s="4">
-        <v>87620</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C110" s="3">
+        <v>53.801140864183132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B111" s="1">
         <v>2013</v>
       </c>
-      <c r="C111" s="4">
-        <v>87652</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C111" s="3">
+        <v>53.820789762923759</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B112" s="1">
         <v>2003</v>
       </c>
-      <c r="C112" s="4">
-        <v>300592</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C112" s="3">
+        <v>164.95198375679087</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B113" s="1">
         <v>2004</v>
       </c>
-      <c r="C113" s="4">
-        <v>275000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C113" s="3">
+        <v>150.90819294298416</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B114" s="1">
         <v>2005</v>
       </c>
-      <c r="C114" s="4">
-        <v>270658</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C114" s="3">
+        <v>148.52548976568073</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B115" s="1">
         <v>2006</v>
       </c>
-      <c r="C115" s="4">
-        <v>258759</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C115" s="3">
+        <v>141.99582944630413</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B116" s="1">
         <v>2007</v>
       </c>
-      <c r="C116" s="4">
-        <v>297916</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C116" s="3">
+        <v>163.48350985018934</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B117" s="1">
         <v>2008</v>
       </c>
-      <c r="C117" s="4">
-        <v>297490</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C117" s="3">
+        <v>163.249739340394</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B118" s="1">
         <v>2009</v>
       </c>
-      <c r="C118" s="4">
-        <v>297490</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C118" s="3">
+        <v>163.249739340394</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B119" s="1">
         <v>2010</v>
       </c>
-      <c r="C119" s="4">
-        <v>265711</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C119" s="3">
+        <v>145.81078856390278</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B120" s="1">
         <v>2011</v>
       </c>
-      <c r="C120" s="4">
-        <v>265801</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C120" s="3">
+        <v>145.86017669977502</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B121" s="1">
         <v>2012</v>
       </c>
-      <c r="C121" s="4">
-        <v>265634</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C121" s="3">
+        <v>145.76853426987873</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B122" s="1">
         <v>2013</v>
       </c>
-      <c r="C122" s="4">
-        <v>258208</v>
+      <c r="C122" s="3">
+        <v>141.6934643033529</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1805,10 +1812,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1818,9 +1830,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>